<commit_message>
Added Serenity Report and Dependencies
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/invalidUserCredentials.xlsx
+++ b/src/main/resources/TestData/invalidUserCredentials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13410" windowHeight="5505"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="4080"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidUserCredentials" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>username</t>
   </si>
@@ -27,9 +27,6 @@
   </si>
   <si>
     <t>invalidUser@vrbank1</t>
-  </si>
-  <si>
-    <t>invalidUser@vrbank2</t>
   </si>
   <si>
     <t>invalidUser@vrbank0</t>
@@ -388,7 +385,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +404,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -422,19 +419,13 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3:A4" r:id="rId2" display="invalidUser@vrbank"/>
     <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="A4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>